<commit_message>
Added new columns in DataBase. Created new Page
</commit_message>
<xml_diff>
--- a/excel/Activity.xlsx
+++ b/excel/Activity.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lisav\Desktop\ConferentionOrganisation\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lisav\Desktop\test\ConferentionOrganisation\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Краткая информация" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="71">
   <si>
     <t>№</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>Activity</t>
+  </si>
+  <si>
+    <t>Direction_Id</t>
   </si>
 </sst>
 </file>
@@ -239,8 +242,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -329,9 +332,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -617,7 +620,7 @@
   </sheetPr>
   <dimension ref="A1:M108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -2251,374 +2254,438 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="98.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="98.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="4">
+        <v>2</v>
+      </c>
+      <c r="D2" s="16">
         <v>44643</v>
       </c>
-      <c r="D2" s="4">
-        <v>2</v>
-      </c>
       <c r="E2" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="4">
+        <v>2</v>
+      </c>
+      <c r="D3" s="16">
         <v>44650</v>
       </c>
-      <c r="D3" s="4">
-        <v>2</v>
-      </c>
       <c r="E3" s="4">
+        <v>2</v>
+      </c>
+      <c r="F3" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="16">
         <v>44620</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E4" s="4">
         <v>3</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F4" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="4">
+        <v>4</v>
+      </c>
+      <c r="D5" s="16">
         <v>45145</v>
       </c>
-      <c r="D5" s="4">
+      <c r="E5" s="4">
         <v>3</v>
       </c>
-      <c r="E5" s="4">
+      <c r="F5" s="4">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="4">
+        <v>5</v>
+      </c>
+      <c r="D6" s="16">
         <v>44672</v>
       </c>
-      <c r="D6" s="4">
-        <v>1</v>
-      </c>
       <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="16">
         <v>44918</v>
       </c>
-      <c r="D7" s="4">
-        <v>2</v>
-      </c>
       <c r="E7" s="4">
+        <v>2</v>
+      </c>
+      <c r="F7" s="4">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="4">
+        <v>3</v>
+      </c>
+      <c r="D8" s="16">
         <v>44581</v>
       </c>
-      <c r="D8" s="4">
-        <v>1</v>
-      </c>
       <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="4">
+        <v>4</v>
+      </c>
+      <c r="D9" s="16">
         <v>45166</v>
       </c>
-      <c r="D9" s="4">
+      <c r="E9" s="4">
         <v>3</v>
       </c>
-      <c r="E9" s="4">
+      <c r="F9" s="4">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="4">
+        <v>4</v>
+      </c>
+      <c r="D10" s="16">
         <v>44680</v>
       </c>
-      <c r="D10" s="4">
+      <c r="E10" s="4">
         <v>3</v>
       </c>
-      <c r="E10" s="4">
+      <c r="F10" s="4">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="4">
+        <v>3</v>
+      </c>
+      <c r="D11" s="16">
         <v>44637</v>
       </c>
-      <c r="D11" s="4">
-        <v>2</v>
-      </c>
       <c r="E11" s="4">
+        <v>2</v>
+      </c>
+      <c r="F11" s="4">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="4">
+        <v>3</v>
+      </c>
+      <c r="D12" s="16">
         <v>44589</v>
       </c>
-      <c r="D12" s="4">
-        <v>1</v>
-      </c>
       <c r="E12" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="F12" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="D13" s="16">
         <v>45026</v>
       </c>
-      <c r="D13" s="4">
+      <c r="E13" s="4">
         <v>3</v>
       </c>
-      <c r="E13" s="4">
+      <c r="F13" s="4">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="4">
+        <v>4</v>
+      </c>
+      <c r="D14" s="16">
         <v>45124</v>
       </c>
-      <c r="D14" s="4">
-        <v>2</v>
-      </c>
       <c r="E14" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="4">
+        <v>4</v>
+      </c>
+      <c r="D15" s="16">
         <v>44786</v>
       </c>
-      <c r="D15" s="4">
+      <c r="E15" s="4">
         <v>3</v>
       </c>
-      <c r="E15" s="4">
+      <c r="F15" s="4">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="4">
+        <v>4</v>
+      </c>
+      <c r="D16" s="16">
         <v>45069</v>
       </c>
-      <c r="D16" s="4">
-        <v>1</v>
-      </c>
       <c r="E16" s="4">
+        <v>1</v>
+      </c>
+      <c r="F16" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="4">
+        <v>4</v>
+      </c>
+      <c r="D17" s="16">
         <v>45145</v>
       </c>
-      <c r="D17" s="4">
-        <v>2</v>
-      </c>
       <c r="E17" s="4">
+        <v>2</v>
+      </c>
+      <c r="F17" s="4">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="4">
+        <v>2</v>
+      </c>
+      <c r="D18" s="16">
         <v>45223</v>
       </c>
-      <c r="D18" s="4">
+      <c r="E18" s="4">
         <v>3</v>
       </c>
-      <c r="E18" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C19" s="4">
+        <v>4</v>
+      </c>
+      <c r="D19" s="16">
         <v>44693</v>
       </c>
-      <c r="D19" s="4">
-        <v>2</v>
-      </c>
       <c r="E19" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="F19" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="16">
+      <c r="C20" s="4">
+        <v>5</v>
+      </c>
+      <c r="D20" s="16">
         <v>45231</v>
       </c>
-      <c r="D20" s="4">
-        <v>2</v>
-      </c>
       <c r="E20" s="4">
+        <v>2</v>
+      </c>
+      <c r="F20" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="16">
+      <c r="C21" s="4">
+        <v>4</v>
+      </c>
+      <c r="D21" s="16">
         <v>44654</v>
       </c>
-      <c r="D21" s="4">
-        <v>2</v>
-      </c>
       <c r="E21" s="4">
+        <v>2</v>
+      </c>
+      <c r="F21" s="4">
         <v>3</v>
       </c>
     </row>

</xml_diff>